<commit_message>
Included 2 method of writing into excel worksheet
</commit_message>
<xml_diff>
--- a/resources/ScrapedInvoiceData.xlsx
+++ b/resources/ScrapedInvoiceData.xlsx
@@ -43,7 +43,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>09/29/2017 00:00:00</x:t>
+    <x:t>09/29/2017</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">1 725,00 
@@ -62,7 +62,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>10/27/2016 00:00:00</x:t>
+    <x:t>10/27/2016</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">650,00 
@@ -81,7 +81,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>08/17/2018 00:00:00</x:t>
+    <x:t>08/17/2018</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">925,00 
@@ -100,7 +100,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>10/07/2017 00:00:00</x:t>
+    <x:t>10/07/2017</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">675,00 
@@ -119,7 +119,7 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>04/06/2016 00:00:00</x:t>
+    <x:t>04/06/2016</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">1 825,00 

</xml_diff>